<commit_message>
Finishing setting up procedural MIDI plugin, Adding glow-on-beat events to grid tiles
</commit_message>
<xml_diff>
--- a/Work log.xlsx
+++ b/Work log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Jonah\Documents\Unreal Projects\Music-Tower-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1958D4BC-C2A6-4A71-8136-5EC666BD58B9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA9E354A-63A8-4C3E-91B1-0B70C0627FB9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>Made Base Classes for Grid, grid blocks, and towers. Added basic pulse visual to start tower</t>
+  </si>
+  <si>
+    <t>Got started on implementing procedural midi plugin</t>
   </si>
 </sst>
 </file>
@@ -359,10 +362,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,6 +402,28 @@
         <v>4</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>43728</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.44027777777777777</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>43729</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.1875</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Moving code to spawn grids from editor from construction script to function call to improve performance and allow editing of grid tile actors. Adding function to spawn default tower from grid tile in editor
</commit_message>
<xml_diff>
--- a/Work log.xlsx
+++ b/Work log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Jonah\Documents\Unreal Projects\Music-Tower-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA9E354A-63A8-4C3E-91B1-0B70C0627FB9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38CC0492-CE6E-44A0-B6C4-63957AF76F19}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>Got started on implementing procedural midi plugin</t>
+  </si>
+  <si>
+    <t>Finished putting in procedural midi plugin, looked into in-engine synthesis, recorded a basic scale and drum beats</t>
+  </si>
+  <si>
+    <t>Changed system for spawning grid tiles from editor, made it so that default towers can be spawned from grid tiles in editor</t>
   </si>
 </sst>
 </file>
@@ -362,10 +368,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,6 +429,26 @@
       <c r="B4" s="2">
         <v>0.1875</v>
       </c>
+      <c r="C4" s="2">
+        <v>0.31041666666666667</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>43729</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.33958333333333335</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.4597222222222222</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>